<commit_message>
updated code for Userlogin DDT for negative and positive(excel)
</commit_message>
<xml_diff>
--- a/src/test/resources/Test_Data/Dietician_testdata.xlsx
+++ b/src/test/resources/Test_Data/Dietician_testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\14044\git\Team4_API\src\test\resources\Test_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E8A73D-8A09-4477-B4D1-CAF9CFA73AB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393617A5-E546-4666-9295-99E5962104F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30" yWindow="750" windowWidth="20460" windowHeight="10770" xr2:uid="{3B040778-FD66-4BD1-8529-4B01D661A3E6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>userLoginEmail</t>
   </si>
@@ -44,23 +44,32 @@
     <t>password</t>
   </si>
   <si>
-    <t>gem@gmail.com</t>
-  </si>
-  <si>
-    <t>sign</t>
-  </si>
-  <si>
     <t>test</t>
   </si>
   <si>
     <t>Team9.admin@gmail.com</t>
+  </si>
+  <si>
+    <t>testing@gmail.com</t>
+  </si>
+  <si>
+    <t>sample</t>
+  </si>
+  <si>
+    <t>scenario</t>
+  </si>
+  <si>
+    <t>Login1</t>
+  </si>
+  <si>
+    <t>Login2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,6 +84,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0080FF"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -98,9 +113,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -436,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3620FDFE-7184-436E-B8B2-5206708222CD}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,34 +464,43 @@
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
+      <c r="C2" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>4</v>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{CE2E955D-1F33-4ED2-901C-449B6873726E}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{7820ED54-4E4D-4D68-A0B8-B9EADFA49EAD}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{7820ED54-4E4D-4D68-A0B8-B9EADFA49EAD}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{1D41FA66-91B7-4EC5-B86C-71FAAB447457}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
working code for both positive and negative userlogin cases using DDT -Excel
</commit_message>
<xml_diff>
--- a/src/test/resources/Test_Data/Dietician_testdata.xlsx
+++ b/src/test/resources/Test_Data/Dietician_testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\14044\git\Team4_API\src\test\resources\Test_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393617A5-E546-4666-9295-99E5962104F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7861154E-87EA-4E28-A575-A40D496E764B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30" yWindow="750" windowWidth="20460" windowHeight="10770" xr2:uid="{3B040778-FD66-4BD1-8529-4B01D661A3E6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t>userLoginEmail</t>
   </si>
@@ -59,10 +59,31 @@
     <t>scenario</t>
   </si>
   <si>
-    <t>Login1</t>
-  </si>
-  <si>
-    <t>Login2</t>
+    <t>LoginPositive1</t>
+  </si>
+  <si>
+    <t>LoginInvalidCredential2</t>
+  </si>
+  <si>
+    <t>LoginInvalidMethod3</t>
+  </si>
+  <si>
+    <t>LoginInvalidEndpoint4</t>
+  </si>
+  <si>
+    <t>LoginInvalidContentType5</t>
+  </si>
+  <si>
+    <t>DieticianLogin6</t>
+  </si>
+  <si>
+    <t>DieticianInvalid7</t>
+  </si>
+  <si>
+    <t>PatientLogin8</t>
+  </si>
+  <si>
+    <t>PatientInvalidLogin9</t>
   </si>
 </sst>
 </file>
@@ -452,16 +473,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3620FDFE-7184-436E-B8B2-5206708222CD}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -482,7 +504,7 @@
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -495,12 +517,68 @@
       </c>
       <c r="C3" s="2" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C10" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{7820ED54-4E4D-4D68-A0B8-B9EADFA49EAD}"/>
     <hyperlink ref="A3" r:id="rId2" xr:uid="{1D41FA66-91B7-4EC5-B86C-71FAAB447457}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{9110D786-EC2C-4324-A938-6976E91F24A8}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{160780AF-4E44-482C-898F-A09CF72B8BC4}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{E8B755D5-7CBF-4979-B5FE-08474A0FCA96}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adding more negative cases and respective code
</commit_message>
<xml_diff>
--- a/src/test/resources/Test_Data/Dietician_testdata.xlsx
+++ b/src/test/resources/Test_Data/Dietician_testdata.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\14044\git\Team4_API\src\test\resources\Test_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sathizk7/eclipse-workspace/Team4_API/src/test/resources/Test_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7861154E-87EA-4E28-A575-A40D496E764B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769AD4C9-B063-C24A-B57B-ECE176991FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="750" windowWidth="20460" windowHeight="10770" xr2:uid="{3B040778-FD66-4BD1-8529-4B01D661A3E6}"/>
+    <workbookView xWindow="5040" yWindow="1500" windowWidth="34500" windowHeight="16380" activeTab="1" xr2:uid="{3B040778-FD66-4BD1-8529-4B01D661A3E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Dietician_data" sheetId="1" r:id="rId1"/>
+    <sheet name="Dietician_Create" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="49">
   <si>
     <t>userLoginEmail</t>
   </si>
@@ -84,12 +85,114 @@
   </si>
   <si>
     <t>PatientInvalidLogin9</t>
+  </si>
+  <si>
+    <t>ContactNumber</t>
+  </si>
+  <si>
+    <t>DateOfBirth</t>
+  </si>
+  <si>
+    <t>Education</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Firstname</t>
+  </si>
+  <si>
+    <t>HospitalCity</t>
+  </si>
+  <si>
+    <t>HospitalName</t>
+  </si>
+  <si>
+    <t>HospitalPincode</t>
+  </si>
+  <si>
+    <t>HospitalStreet</t>
+  </si>
+  <si>
+    <t>Lastname</t>
+  </si>
+  <si>
+    <t>bachelors</t>
+  </si>
+  <si>
+    <t>apple</t>
+  </si>
+  <si>
+    <t>chennai</t>
+  </si>
+  <si>
+    <t>malar</t>
+  </si>
+  <si>
+    <t>big street</t>
+  </si>
+  <si>
+    <t>orange</t>
+  </si>
+  <si>
+    <t>create_dietician_invalidData</t>
+  </si>
+  <si>
+    <t>diet23@ninja.com</t>
+  </si>
+  <si>
+    <t>7123661a58</t>
+  </si>
+  <si>
+    <t>Invalid_Data</t>
+  </si>
+  <si>
+    <t>invalid_Contact_number</t>
+  </si>
+  <si>
+    <t>invalid_DOB</t>
+  </si>
+  <si>
+    <t>apple1</t>
+  </si>
+  <si>
+    <t>orange!</t>
+  </si>
+  <si>
+    <t>invalid_FirstName</t>
+  </si>
+  <si>
+    <t>invalid_LastName</t>
+  </si>
+  <si>
+    <t>diet23@ninjacom</t>
+  </si>
+  <si>
+    <t>invalid_Email</t>
+  </si>
+  <si>
+    <t>invalid_Education</t>
+  </si>
+  <si>
+    <t>invalid_HospitalPincode</t>
+  </si>
+  <si>
+    <t>invalid_HospitalCity</t>
+  </si>
+  <si>
+    <t>chennai1+</t>
+  </si>
+  <si>
+    <t>bachelors$25</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -134,10 +237,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -475,18 +587,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3620FDFE-7184-436E-B8B2-5206708222CD}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -497,7 +609,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -508,7 +620,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -519,7 +631,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -530,7 +642,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -541,7 +653,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -552,22 +664,22 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C8" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C9" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C10" s="2" t="s">
         <v>15</v>
       </c>
@@ -582,4 +694,376 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB87BE5E-98A9-C441-BDF7-E62B8C946D47}">
+  <dimension ref="A1:L9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="10" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="5">
+        <v>45499</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="3">
+        <v>600050</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>7123661858</v>
+      </c>
+      <c r="B3" s="5">
+        <v>45499</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="3">
+        <v>600050</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>7123661858</v>
+      </c>
+      <c r="B4" s="5">
+        <v>45499</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="3">
+        <v>600050</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>7123661858</v>
+      </c>
+      <c r="B5" s="5">
+        <v>45499</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="3">
+        <v>60050</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>5823661858</v>
+      </c>
+      <c r="B6" s="5">
+        <v>38194</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="3">
+        <v>60050</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>7145061858</v>
+      </c>
+      <c r="B7" s="5">
+        <v>41846</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="3">
+        <v>600050</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <v>7130261858</v>
+      </c>
+      <c r="B8" s="5">
+        <v>41116</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="3">
+        <v>600050</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>7122861058</v>
+      </c>
+      <c r="B9" s="3">
+        <v>12</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" s="3">
+        <v>600050</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{B29F70AA-40E3-3843-BAF0-E080311B37E3}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{AA260715-6E7C-1047-B8DF-8CA17073DC0C}"/>
+    <hyperlink ref="D5" r:id="rId3" xr:uid="{149609E4-D429-4D46-9B67-FD9A4E702DF2}"/>
+    <hyperlink ref="D9" r:id="rId4" xr:uid="{396DC42D-501E-5948-8970-2EE8A1696595}"/>
+    <hyperlink ref="D3" r:id="rId5" xr:uid="{72BAC8B4-2142-7B42-9039-5FADC4525B19}"/>
+    <hyperlink ref="D8" r:id="rId6" xr:uid="{0C3C9B61-9430-384C-B946-B601E130C846}"/>
+    <hyperlink ref="D7" r:id="rId7" xr:uid="{41B61D21-6725-3D46-814D-723394493636}"/>
+    <hyperlink ref="D6" r:id="rId8" xr:uid="{77B18B4B-D71A-EF45-9D85-3A128792B319}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
modified login code and added logout feature
</commit_message>
<xml_diff>
--- a/src/test/resources/Test_Data/Dietician_testdata.xlsx
+++ b/src/test/resources/Test_Data/Dietician_testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sathizk7/eclipse-workspace/Team4_API/src/test/resources/Test_Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\14044\git\Team4_API\src\test\resources\Test_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769AD4C9-B063-C24A-B57B-ECE176991FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AED6FAC-88E0-4522-A5EB-F25EAC8008FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5040" yWindow="1500" windowWidth="34500" windowHeight="16380" activeTab="1" xr2:uid="{3B040778-FD66-4BD1-8529-4B01D661A3E6}"/>
+    <workbookView xWindow="30" yWindow="750" windowWidth="20460" windowHeight="10770" xr2:uid="{3B040778-FD66-4BD1-8529-4B01D661A3E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Dietician_data" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="53">
   <si>
     <t>userLoginEmail</t>
   </si>
@@ -75,18 +75,6 @@
     <t>LoginInvalidContentType5</t>
   </si>
   <si>
-    <t>DieticianLogin6</t>
-  </si>
-  <si>
-    <t>DieticianInvalid7</t>
-  </si>
-  <si>
-    <t>PatientLogin8</t>
-  </si>
-  <si>
-    <t>PatientInvalidLogin9</t>
-  </si>
-  <si>
     <t>ContactNumber</t>
   </si>
   <si>
@@ -184,6 +172,30 @@
   </si>
   <si>
     <t>bachelors$25</t>
+  </si>
+  <si>
+    <t>PatientLogin1</t>
+  </si>
+  <si>
+    <t>patient</t>
+  </si>
+  <si>
+    <t>patient@html</t>
+  </si>
+  <si>
+    <t>PatientInvalidLogin2</t>
+  </si>
+  <si>
+    <t>DieticianInvalid2</t>
+  </si>
+  <si>
+    <t>ignore@yahoo</t>
+  </si>
+  <si>
+    <t>dietician</t>
+  </si>
+  <si>
+    <t>DieticianLogin1</t>
   </si>
 </sst>
 </file>
@@ -193,7 +205,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,6 +224,12 @@
     <font>
       <sz val="10"/>
       <color rgb="FF0080FF"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF2A00FF"/>
       <name val="Courier New"/>
       <family val="3"/>
     </font>
@@ -237,7 +255,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -250,6 +268,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -585,20 +604,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3620FDFE-7184-436E-B8B2-5206708222CD}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -609,7 +628,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -620,7 +639,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -631,7 +650,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -642,7 +661,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -653,7 +672,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -664,25 +683,47 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>51</v>
+      </c>
       <c r="C8" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
       <c r="C9" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
       <c r="C10" s="2" t="s">
-        <v>15</v>
-      </c>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C12" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -691,6 +732,8 @@
     <hyperlink ref="A4" r:id="rId3" xr:uid="{9110D786-EC2C-4324-A938-6976E91F24A8}"/>
     <hyperlink ref="A5" r:id="rId4" xr:uid="{160780AF-4E44-482C-898F-A09CF72B8BC4}"/>
     <hyperlink ref="A6" r:id="rId5" xr:uid="{E8B755D5-7CBF-4979-B5FE-08474A0FCA96}"/>
+    <hyperlink ref="A10" r:id="rId6" xr:uid="{E8E52803-F5D0-49FB-8CA8-BB059F26A3C2}"/>
+    <hyperlink ref="A8" r:id="rId7" xr:uid="{BC9B24F4-FE8D-4537-82C4-9346506EC3AF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -700,94 +743,94 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB87BE5E-98A9-C441-BDF7-E62B8C946D47}">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="10.83203125" style="3"/>
+    <col min="1" max="1" width="11.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="10" width="10.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="K1" t="s">
         <v>6</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B2" s="5">
         <v>45499</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H2" s="3">
         <v>600050</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="K2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="L2" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>7123661858</v>
       </c>
@@ -795,37 +838,37 @@
         <v>45499</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H3" s="3">
         <v>600050</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>7123661858</v>
       </c>
@@ -833,37 +876,37 @@
         <v>45499</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H4" s="3">
         <v>600050</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>7123661858</v>
       </c>
@@ -871,37 +914,37 @@
         <v>45499</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H5" s="3">
         <v>60050</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5823661858</v>
       </c>
@@ -909,37 +952,37 @@
         <v>38194</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H6" s="3">
         <v>60050</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>7145061858</v>
       </c>
@@ -947,37 +990,37 @@
         <v>41846</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H7" s="3">
         <v>600050</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7130261858</v>
       </c>
@@ -985,37 +1028,37 @@
         <v>41116</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H8" s="3">
         <v>600050</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>7122861058</v>
       </c>
@@ -1023,34 +1066,34 @@
         <v>12</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H9" s="3">
         <v>600050</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding additional details scenario and their code and test data
</commit_message>
<xml_diff>
--- a/src/test/resources/Test_Data/Dietician_testdata.xlsx
+++ b/src/test/resources/Test_Data/Dietician_testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sathizk7/eclipse-workspace/Team4_API/src/test/resources/Test_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769AD4C9-B063-C24A-B57B-ECE176991FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C22A26FF-86B8-4044-BC07-53C3CFEB6D87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5040" yWindow="1500" windowWidth="34500" windowHeight="16380" activeTab="1" xr2:uid="{3B040778-FD66-4BD1-8529-4B01D661A3E6}"/>
+    <workbookView xWindow="3900" yWindow="1500" windowWidth="34500" windowHeight="16380" activeTab="1" xr2:uid="{3B040778-FD66-4BD1-8529-4B01D661A3E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Dietician_data" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="55">
   <si>
     <t>userLoginEmail</t>
   </si>
@@ -184,6 +184,24 @@
   </si>
   <si>
     <t>bachelors$25</t>
+  </si>
+  <si>
+    <t>Middlename</t>
+  </si>
+  <si>
+    <t>SecondaryContact</t>
+  </si>
+  <si>
+    <t>numpy</t>
+  </si>
+  <si>
+    <t>valid_additional_data</t>
+  </si>
+  <si>
+    <t>invalid_additional_data</t>
+  </si>
+  <si>
+    <t>create_dietician_AdditionalData</t>
   </si>
 </sst>
 </file>
@@ -698,20 +716,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB87BE5E-98A9-C441-BDF7-E62B8C946D47}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="10.83203125" style="3"/>
+    <col min="3" max="11" width="10.83203125" style="3"/>
+    <col min="12" max="12" width="11.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.83203125" customWidth="1"/>
+    <col min="14" max="14" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
@@ -742,14 +763,20 @@
       <c r="J1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="M1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>34</v>
       </c>
@@ -780,14 +807,14 @@
       <c r="J2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>7123661858</v>
       </c>
@@ -818,14 +845,14 @@
       <c r="J3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>7123661858</v>
       </c>
@@ -856,14 +883,14 @@
       <c r="J4" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>7123661858</v>
       </c>
@@ -894,14 +921,14 @@
       <c r="J5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="M5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="N5" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>5823661858</v>
       </c>
@@ -924,7 +951,7 @@
         <v>29</v>
       </c>
       <c r="H6" s="3">
-        <v>60050</v>
+        <v>600050</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>30</v>
@@ -932,14 +959,14 @@
       <c r="J6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="M6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="N6" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>7145061858</v>
       </c>
@@ -970,14 +997,14 @@
       <c r="J7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="M7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="N7" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>7130261858</v>
       </c>
@@ -1008,14 +1035,14 @@
       <c r="J8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="M8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="N8" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>7122861058</v>
       </c>
@@ -1046,11 +1073,39 @@
       <c r="J9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="M9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="N9" s="3" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+      <c r="K10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="L10" s="3">
+        <v>8456798123</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+      <c r="K11" s="3">
+        <v>123</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>